<commit_message>
sempre tem mais conserto
</commit_message>
<xml_diff>
--- a/Codificação.xlsx
+++ b/Codificação.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>add</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>NOT((F(5) AND F(2) OR NOT F(5) AND F(3) OR NOT F(5) AND F(1)) AND AO1)</t>
+  </si>
+  <si>
+    <t>AC4</t>
+  </si>
+  <si>
+    <t>AC4 =</t>
+  </si>
+  <si>
+    <t>NOT(AND F(i), i in 0..1) AND AO1</t>
   </si>
 </sst>
 </file>
@@ -176,11 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +483,7 @@
     <col min="8" max="13" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -499,19 +509,22 @@
         <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -542,7 +555,7 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="4">
         <v>0</v>
       </c>
       <c r="L2" s="3">
@@ -551,8 +564,11 @@
       <c r="M2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -583,17 +599,20 @@
       <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="4">
         <v>0</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -624,17 +643,20 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -665,17 +687,20 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
-        <v>1</v>
+      <c r="K5" s="4">
+        <v>0</v>
       </c>
       <c r="L5" s="3">
         <v>1</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -706,8 +731,8 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
-        <v>1</v>
+      <c r="K6" s="4">
+        <v>0</v>
       </c>
       <c r="L6" s="3">
         <v>1</v>
@@ -715,8 +740,11 @@
       <c r="M6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -745,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
       </c>
       <c r="L7" s="3">
         <v>0</v>
@@ -756,8 +784,11 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -788,17 +819,20 @@
       <c r="J8" s="1">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
-        <v>1</v>
+      <c r="K8" s="4">
+        <v>0</v>
       </c>
       <c r="L8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -829,17 +863,20 @@
       <c r="J9" s="1">
         <v>1</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="4">
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -870,17 +907,20 @@
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="4">
         <v>0</v>
       </c>
       <c r="L10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -911,17 +951,20 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="4">
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -952,17 +995,20 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="4">
         <v>0</v>
       </c>
       <c r="L12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -993,39 +1039,36 @@
       <c r="J13" s="1">
         <v>0</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="4">
         <v>0</v>
       </c>
       <c r="L13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -1033,35 +1076,49 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>26</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>